<commit_message>
FINALIZED THE FINAL VERSION OF THE PROJECT
</commit_message>
<xml_diff>
--- a/foodsales.xlsx
+++ b/foodsales.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr codeName="ThisWorkbook" showPivotChartFilter="1" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\VSC\app-dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09217CA4-2E96-4840-BD5F-E399AB240614}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3006E42-3ED0-41A8-B78F-ACAA0D597F51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FoodSales" sheetId="16" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="17" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -803,7 +805,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:J245"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="M8" sqref="M8"/>
     </sheetView>
@@ -7447,4 +7449,16 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E709D6A-515C-494D-B554-3D14F7CB0B04}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>